<commit_message>
Array Save to DB
</commit_message>
<xml_diff>
--- a/BuildDBScript/JsonToExcel.xlsx
+++ b/BuildDBScript/JsonToExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SNNBFailover\BuildDBScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AF3503-177B-4F8D-B6C2-0028CFB850F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D66E1C7-C0F7-44C6-887B-CA7B0E451E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42780" yWindow="0" windowWidth="18660" windowHeight="17280" firstSheet="2" activeTab="3" xr2:uid="{2B70F1A1-21A2-4A0E-AB73-14BC681AD4F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="3" xr2:uid="{2B70F1A1-21A2-4A0E-AB73-14BC681AD4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="3" r:id="rId1"/>
@@ -1174,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1188,11 +1188,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1203,15 +1199,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="51">
-    <dxf>
-      <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1237,10 +1224,7 @@
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1257,6 +1241,18 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1635,12 +1631,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{24D814A6-1CEC-4AEF-A328-1CD2A4C08D6D}" name="Table_RfOutputStream" displayName="Table_RfOutputStream" ref="A1:N41" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:N41" xr:uid="{24D814A6-1CEC-4AEF-A328-1CD2A4C08D6D}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6063A3EA-E7ED-4664-BF1B-624A18D1981A}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6063A3EA-E7ED-4664-BF1B-624A18D1981A}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{5F6B9E3D-F6C7-41AB-882E-AEEB01CAA7DC}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{67043735-9D1F-4EFE-BE83-85CA3E2F8AE6}" uniqueName="3" name="Value.value" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{03F9C369-B02B-4E0A-B585-F38103A75F93}" uniqueName="4" name="StringLength" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{5DE39BA3-6B32-4E50-A22A-80B30B6DCC7C}" uniqueName="5" name="Access" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{1BDDE075-F09B-4795-B56C-0020089F2C9B}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{1BDDE075-F09B-4795-B56C-0020089F2C9B}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{DAA22772-FC2A-48E9-8EBD-CF0174760F01}" uniqueName="7" name="Scale" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{5C79966D-28ED-4B38-8DEF-162DF486CF52}" uniqueName="8" name="Format" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{A3495477-A5CF-401C-970E-7C9F91DAF030}" uniqueName="9" name="Units" queryTableFieldId="9"/>
@@ -1648,7 +1644,7 @@
       <calculatedColumnFormula>UPPER(LEFT(A2,1))&amp;RIGHT(A2,LEN(A2)-1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{03F8C291-A5D6-4518-BDCE-64E83A803BF4}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11">
-      <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value;"))</calculatedColumnFormula>
+      <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = restMain.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = restMain.", A2, ".value;"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{E08D0890-1A9D-4197-8D95-A64C2D03F892}" uniqueName="12" name="Include" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{3F92766F-9297-40A6-B1FC-6A4337C73240}" uniqueName="13" name="Type translate" queryTableFieldId="13">
@@ -1678,26 +1674,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}" name="Table_RfInputStream" displayName="Table_RfInputStream" ref="A1:N20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}" name="Table_RfInputStream" displayName="Table_RfInputStream" ref="A1:N20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:N20" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{485F7603-3220-49DD-B3CE-BFD08F35B4F8}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{321E942D-A13D-4AF0-AA77-E3500F5EB193}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{18F13399-7530-4051-8061-5D3623022EC1}" uniqueName="3" name="Value.value" queryTableFieldId="3" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{8F5EA99F-A1D5-4DCA-9D86-CE635CE023A7}" uniqueName="4" name="StringLength" queryTableFieldId="4" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{43FAB6A3-A2E3-48D6-B09C-12B3A53D6D11}" uniqueName="5" name="Access" queryTableFieldId="5" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{522604AD-37CB-4F5E-8E4D-89F1B491602D}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E561D537-D6AB-4F01-90DA-3BB8AB928187}" uniqueName="7" name="Scale" queryTableFieldId="7" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{106A1A6F-1D11-4875-B000-BA1B53D0CF4C}" uniqueName="8" name="Format" queryTableFieldId="8" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{84AF41AD-5261-4D2A-BC8C-68C1F8B88E4A}" uniqueName="9" name="Units" queryTableFieldId="9" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{9E5BB20E-C3F2-46F6-B5EA-7E078EB418AE}" uniqueName="10" name="CapName" queryTableFieldId="10" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{485F7603-3220-49DD-B3CE-BFD08F35B4F8}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{321E942D-A13D-4AF0-AA77-E3500F5EB193}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{18F13399-7530-4051-8061-5D3623022EC1}" uniqueName="3" name="Value.value" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{8F5EA99F-A1D5-4DCA-9D86-CE635CE023A7}" uniqueName="4" name="StringLength" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{43FAB6A3-A2E3-48D6-B09C-12B3A53D6D11}" uniqueName="5" name="Access" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{522604AD-37CB-4F5E-8E4D-89F1B491602D}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{E561D537-D6AB-4F01-90DA-3BB8AB928187}" uniqueName="7" name="Scale" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{106A1A6F-1D11-4875-B000-BA1B53D0CF4C}" uniqueName="8" name="Format" queryTableFieldId="8" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{84AF41AD-5261-4D2A-BC8C-68C1F8B88E4A}" uniqueName="9" name="Units" queryTableFieldId="9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{9E5BB20E-C3F2-46F6-B5EA-7E078EB418AE}" uniqueName="10" name="CapName" queryTableFieldId="10" dataDxfId="4">
       <calculatedColumnFormula>UPPER(LEFT(A2,1))&amp;RIGHT(A2,LEN(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D10744BC-3808-4F25-B3AB-2402E774E707}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{D10744BC-3808-4F25-B3AB-2402E774E707}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value;"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8219D72E-B8A2-402F-8D09-24C87022E783}" uniqueName="12" name="Include" queryTableFieldId="12" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{644B8F5D-451A-40B4-8939-D1515D745218}" uniqueName="13" name="Type translate" queryTableFieldId="13" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{8219D72E-B8A2-402F-8D09-24C87022E783}" uniqueName="12" name="Include" queryTableFieldId="12" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{644B8F5D-451A-40B4-8939-D1515D745218}" uniqueName="13" name="Type translate" queryTableFieldId="13" dataDxfId="1">
       <calculatedColumnFormula>IF(B2 = "uint8", "[NUMERIC](5) NOT NULL,",
  IF(B2 = "uint16", "[NUMERIC](5) NOT NULL,",
  IF(B2 = "uint32", "[NUMERIC](10) NOT NULL,",
@@ -1715,7 +1711,7 @@
  IF(B2 = "image", "[Image] NOT NULL,",
 "")))))))))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{9EB1E7BC-2297-4F8F-B325-B0E00FD1A8AF}" uniqueName="14" name="Sql Script" queryTableFieldId="14" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{9EB1E7BC-2297-4F8F-B325-B0E00FD1A8AF}" uniqueName="14" name="Sql Script" queryTableFieldId="14" dataDxfId="0">
       <calculatedColumnFormula>IF(L2=FALSE,"",_xlfn.CONCAT("[",A2,"] ", M2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6084,7 +6080,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K2" sqref="K2:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6093,7 +6089,7 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8"/>
+    <col min="6" max="6" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -6141,7 +6137,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>241</v>
       </c>
       <c r="B2" t="s">
@@ -6167,8 +6163,8 @@
         <v>Name</v>
       </c>
       <c r="K2" s="2" t="str">
-        <f xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = sNWBRest.rootObject.", A2, ".value;"))</f>
-        <v>this.Name = sNWBRest.rootObject.name.value.Truncate( 128);</v>
+        <f xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = restMain.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = restMain.", A2, ".value;"))</f>
+        <v>this.Name = restMain.name.value.Truncate( 128);</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>
@@ -6198,7 +6194,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>286</v>
       </c>
       <c r="B3" t="s">
@@ -6210,7 +6206,7 @@
       <c r="E3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>317</v>
       </c>
       <c r="G3">
@@ -6227,8 +6223,8 @@
         <v>CurrentBuffer</v>
       </c>
       <c r="K3" s="2" t="str">
-        <f t="shared" ref="K3:K41" si="1" xml:space="preserve"> IF(B3 = "string", _xlfn.CONCAT("this.", J3, " = sNWBRest.rootObject.", A3, ".value.Truncate( ", D3, ");"), _xlfn.CONCAT("this.", J3, " = sNWBRest.rootObject.", A3, ".value;"))</f>
-        <v>this.CurrentBuffer = sNWBRest.rootObject.currentBuffer.value;</v>
+        <f t="shared" ref="K3:K41" si="1" xml:space="preserve"> IF(B3 = "string", _xlfn.CONCAT("this.", J3, " = restMain.", A3, ".value.Truncate( ", D3, ");"), _xlfn.CONCAT("this.", J3, " = restMain.", A3, ".value;"))</f>
+        <v>this.CurrentBuffer = restMain.currentBuffer.value;</v>
       </c>
       <c r="L3" s="2" t="b">
         <v>1</v>
@@ -6258,7 +6254,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>243</v>
       </c>
       <c r="B4" t="s">
@@ -6270,7 +6266,7 @@
       <c r="E4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>265</v>
       </c>
       <c r="J4" s="2" t="str">
@@ -6279,7 +6275,7 @@
       </c>
       <c r="K4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DataSampleWidth = sNWBRest.rootObject.dataSampleWidth.value;</v>
+        <v>this.DataSampleWidth = restMain.dataSampleWidth.value;</v>
       </c>
       <c r="L4" s="2" t="b">
         <v>1</v>
@@ -6294,7 +6290,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>287</v>
       </c>
       <c r="B5" t="s">
@@ -6306,7 +6302,7 @@
       <c r="E5" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>318</v>
       </c>
       <c r="J5" s="2" t="str">
@@ -6315,7 +6311,7 @@
       </c>
       <c r="K5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DataSource = sNWBRest.rootObject.dataSource.value.Truncate( );</v>
+        <v>this.DataSource = restMain.dataSource.value.Truncate( );</v>
       </c>
       <c r="L5" s="2" t="b">
         <v>1</v>
@@ -6330,7 +6326,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>289</v>
       </c>
       <c r="B6" t="s">
@@ -6342,7 +6338,7 @@
       <c r="E6" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>319</v>
       </c>
       <c r="G6">
@@ -6360,7 +6356,7 @@
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DesiredBuffer = sNWBRest.rootObject.desiredBuffer.value;</v>
+        <v>this.DesiredBuffer = restMain.desiredBuffer.value;</v>
       </c>
       <c r="L6" s="2" t="b">
         <v>1</v>
@@ -6375,7 +6371,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>290</v>
       </c>
       <c r="B7" t="s">
@@ -6387,7 +6383,7 @@
       <c r="E7" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>320</v>
       </c>
       <c r="G7">
@@ -6405,7 +6401,7 @@
       </c>
       <c r="K7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DesiredDelay = sNWBRest.rootObject.desiredDelay.value;</v>
+        <v>this.DesiredDelay = restMain.desiredDelay.value;</v>
       </c>
       <c r="L7" s="2" t="b">
         <v>1</v>
@@ -6420,7 +6416,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>246</v>
       </c>
       <c r="B8" t="s">
@@ -6432,7 +6428,7 @@
       <c r="E8" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>321</v>
       </c>
       <c r="J8" s="2" t="str">
@@ -6441,7 +6437,7 @@
       </c>
       <c r="K8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DestinationPort = sNWBRest.rootObject.destinationPort.value;</v>
+        <v>this.DestinationPort = restMain.destinationPort.value;</v>
       </c>
       <c r="L8" s="2" t="b">
         <v>1</v>
@@ -6456,7 +6452,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>291</v>
       </c>
       <c r="B9" t="s">
@@ -6468,7 +6464,7 @@
       <c r="E9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>322</v>
       </c>
       <c r="J9" s="2" t="str">
@@ -6477,7 +6473,7 @@
       </c>
       <c r="K9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.DroppedPackets = sNWBRest.rootObject.droppedPackets.value;</v>
+        <v>this.DroppedPackets = restMain.droppedPackets.value;</v>
       </c>
       <c r="L9" s="2" t="b">
         <v>1</v>
@@ -6492,7 +6488,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>247</v>
       </c>
       <c r="B10" t="s">
@@ -6504,7 +6500,7 @@
       <c r="E10" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>268</v>
       </c>
       <c r="G10">
@@ -6522,7 +6518,7 @@
       </c>
       <c r="K10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.FrequencyOffset = sNWBRest.rootObject.frequencyOffset.value;</v>
+        <v>this.FrequencyOffset = restMain.frequencyOffset.value;</v>
       </c>
       <c r="L10" s="2" t="b">
         <v>1</v>
@@ -6537,7 +6533,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>292</v>
       </c>
       <c r="B11" t="s">
@@ -6549,7 +6545,7 @@
       <c r="E11" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>323</v>
       </c>
       <c r="J11" s="2" t="str">
@@ -6558,7 +6554,7 @@
       </c>
       <c r="K11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.GapCount = sNWBRest.rootObject.gapCount.value;</v>
+        <v>this.GapCount = restMain.gapCount.value;</v>
       </c>
       <c r="L11" s="2" t="b">
         <v>1</v>
@@ -6573,7 +6569,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>293</v>
       </c>
       <c r="B12" t="s">
@@ -6585,7 +6581,7 @@
       <c r="E12" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>324</v>
       </c>
       <c r="G12">
@@ -6603,7 +6599,7 @@
       </c>
       <c r="K12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.MeasuredDelay = sNWBRest.rootObject.measuredDelay.value;</v>
+        <v>this.MeasuredDelay = restMain.measuredDelay.value;</v>
       </c>
       <c r="L12" s="2" t="b">
         <v>1</v>
@@ -6618,7 +6614,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>250</v>
       </c>
       <c r="B13" t="s">
@@ -6630,7 +6626,7 @@
       <c r="E13" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>325</v>
       </c>
       <c r="G13">
@@ -6648,7 +6644,7 @@
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.MeasuredNetworkRate = sNWBRest.rootObject.measuredNetworkRate.value;</v>
+        <v>this.MeasuredNetworkRate = restMain.measuredNetworkRate.value;</v>
       </c>
       <c r="L13" s="2" t="b">
         <v>1</v>
@@ -6663,7 +6659,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>252</v>
       </c>
       <c r="B14" t="s">
@@ -6675,7 +6671,7 @@
       <c r="E14" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>326</v>
       </c>
       <c r="G14">
@@ -6693,7 +6689,7 @@
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.MeasuredPacketRate = sNWBRest.rootObject.measuredPacketRate.value;</v>
+        <v>this.MeasuredPacketRate = restMain.measuredPacketRate.value;</v>
       </c>
       <c r="L14" s="2" t="b">
         <v>1</v>
@@ -6708,7 +6704,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>294</v>
       </c>
       <c r="B15" t="s">
@@ -6720,7 +6716,7 @@
       <c r="E15" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="6" t="s">
         <v>327</v>
       </c>
       <c r="J15" s="2" t="str">
@@ -6729,7 +6725,7 @@
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.NetStreamGain = sNWBRest.rootObject.netStreamGain.value;</v>
+        <v>this.NetStreamGain = restMain.netStreamGain.value;</v>
       </c>
       <c r="L15" s="2" t="b">
         <v>1</v>
@@ -6744,7 +6740,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>295</v>
       </c>
       <c r="B16" t="s">
@@ -6756,7 +6752,7 @@
       <c r="E16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>328</v>
       </c>
       <c r="G16">
@@ -6774,7 +6770,7 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.NetworkDelay = sNWBRest.rootObject.networkDelay.value;</v>
+        <v>this.NetworkDelay = restMain.networkDelay.value;</v>
       </c>
       <c r="L16" s="2" t="b">
         <v>1</v>
@@ -6789,7 +6785,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>254</v>
       </c>
       <c r="B17" t="s">
@@ -6801,7 +6797,7 @@
       <c r="E17" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>275</v>
       </c>
       <c r="I17" t="s">
@@ -6813,7 +6809,7 @@
       </c>
       <c r="K17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PacketOverhead = sNWBRest.rootObject.packetOverhead.value;</v>
+        <v>this.PacketOverhead = restMain.packetOverhead.value;</v>
       </c>
       <c r="L17" s="2" t="b">
         <v>1</v>
@@ -6828,7 +6824,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>296</v>
       </c>
       <c r="B18" t="s">
@@ -6840,7 +6836,7 @@
       <c r="E18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>329</v>
       </c>
       <c r="J18" s="2" t="str">
@@ -6849,7 +6845,7 @@
       </c>
       <c r="K18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PfecDecoderStatus = sNWBRest.rootObject.pfecDecoderStatus.value.Truncate( );</v>
+        <v>this.PfecDecoderStatus = restMain.pfecDecoderStatus.value.Truncate( );</v>
       </c>
       <c r="L18" s="2" t="b">
         <v>1</v>
@@ -6864,7 +6860,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
         <v>298</v>
       </c>
       <c r="B19" t="s">
@@ -6876,7 +6872,7 @@
       <c r="E19" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>330</v>
       </c>
       <c r="J19" s="2" t="str">
@@ -6885,7 +6881,7 @@
       </c>
       <c r="K19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PfecMissingSets = sNWBRest.rootObject.pfecMissingSets.value;</v>
+        <v>this.PfecMissingSets = restMain.pfecMissingSets.value;</v>
       </c>
       <c r="L19" s="2" t="b">
         <v>1</v>
@@ -6900,7 +6896,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>299</v>
       </c>
       <c r="B20" t="s">
@@ -6912,7 +6908,7 @@
       <c r="E20" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>331</v>
       </c>
       <c r="J20" s="2" t="str">
@@ -6921,7 +6917,7 @@
       </c>
       <c r="K20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PfecRepairedPackets = sNWBRest.rootObject.pfecRepairedPackets.value;</v>
+        <v>this.PfecRepairedPackets = restMain.pfecRepairedPackets.value;</v>
       </c>
       <c r="L20" s="2" t="b">
         <v>1</v>
@@ -6936,7 +6932,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
         <v>300</v>
       </c>
       <c r="B21" t="s">
@@ -6948,7 +6944,7 @@
       <c r="E21" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>332</v>
       </c>
       <c r="J21" s="2" t="str">
@@ -6957,7 +6953,7 @@
       </c>
       <c r="K21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PfecTotalPackets = sNWBRest.rootObject.pfecTotalPackets.value;</v>
+        <v>this.PfecTotalPackets = restMain.pfecTotalPackets.value;</v>
       </c>
       <c r="L21" s="2" t="b">
         <v>1</v>
@@ -6972,7 +6968,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>301</v>
       </c>
       <c r="B22" t="s">
@@ -6984,7 +6980,7 @@
       <c r="E22" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="6" t="s">
         <v>333</v>
       </c>
       <c r="J22" s="2" t="str">
@@ -6993,7 +6989,7 @@
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PfecUnrepairablePackets = sNWBRest.rootObject.pfecUnrepairablePackets.value;</v>
+        <v>this.PfecUnrepairablePackets = restMain.pfecUnrepairablePackets.value;</v>
       </c>
       <c r="L22" s="2" t="b">
         <v>1</v>
@@ -7008,7 +7004,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" t="s">
         <v>302</v>
       </c>
       <c r="B23" t="s">
@@ -7020,7 +7016,7 @@
       <c r="E23" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="6" t="s">
         <v>334</v>
       </c>
       <c r="J23" s="2" t="str">
@@ -7029,7 +7025,7 @@
       </c>
       <c r="K23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatency = sNWBRest.rootObject.preserveLatency.value;</v>
+        <v>this.PreserveLatency = restMain.preserveLatency.value;</v>
       </c>
       <c r="L23" s="2" t="b">
         <v>1</v>
@@ -7044,7 +7040,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
         <v>303</v>
       </c>
       <c r="B24" t="s">
@@ -7056,7 +7052,7 @@
       <c r="E24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="6" t="s">
         <v>335</v>
       </c>
       <c r="J24" s="2" t="str">
@@ -7065,7 +7061,7 @@
       </c>
       <c r="K24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatencyLatePackets = sNWBRest.rootObject.preserveLatencyLatePackets.value;</v>
+        <v>this.PreserveLatencyLatePackets = restMain.preserveLatencyLatePackets.value;</v>
       </c>
       <c r="L24" s="2" t="b">
         <v>1</v>
@@ -7080,7 +7076,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
         <v>304</v>
       </c>
       <c r="B25" t="s">
@@ -7092,7 +7088,7 @@
       <c r="E25" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="6" t="s">
         <v>336</v>
       </c>
       <c r="J25" s="2" t="str">
@@ -7101,7 +7097,7 @@
       </c>
       <c r="K25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatencyMaxBurstLoss = sNWBRest.rootObject.preserveLatencyMaxBurstLoss.value;</v>
+        <v>this.PreserveLatencyMaxBurstLoss = restMain.preserveLatencyMaxBurstLoss.value;</v>
       </c>
       <c r="L25" s="2" t="b">
         <v>1</v>
@@ -7116,7 +7112,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>305</v>
       </c>
       <c r="B26" t="s">
@@ -7128,7 +7124,7 @@
       <c r="E26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>337</v>
       </c>
       <c r="J26" s="2" t="str">
@@ -7137,7 +7133,7 @@
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatencyMissingPackets = sNWBRest.rootObject.preserveLatencyMissingPackets.value;</v>
+        <v>this.PreserveLatencyMissingPackets = restMain.preserveLatencyMissingPackets.value;</v>
       </c>
       <c r="L26" s="2" t="b">
         <v>1</v>
@@ -7152,7 +7148,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
         <v>306</v>
       </c>
       <c r="B27" t="s">
@@ -7164,7 +7160,7 @@
       <c r="E27" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>338</v>
       </c>
       <c r="J27" s="2" t="str">
@@ -7173,7 +7169,7 @@
       </c>
       <c r="K27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatencyOutOfOrderPackets = sNWBRest.rootObject.preserveLatencyOutOfOrderPackets.value;</v>
+        <v>this.PreserveLatencyOutOfOrderPackets = restMain.preserveLatencyOutOfOrderPackets.value;</v>
       </c>
       <c r="L27" s="2" t="b">
         <v>1</v>
@@ -7188,7 +7184,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" t="s">
         <v>307</v>
       </c>
       <c r="B28" t="s">
@@ -7200,7 +7196,7 @@
       <c r="E28" t="s">
         <v>136</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="6" t="s">
         <v>339</v>
       </c>
       <c r="I28" t="s">
@@ -7212,7 +7208,7 @@
       </c>
       <c r="K28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.PreserveLatencyReleaseMargin = sNWBRest.rootObject.preserveLatencyReleaseMargin.value;</v>
+        <v>this.PreserveLatencyReleaseMargin = restMain.preserveLatencyReleaseMargin.value;</v>
       </c>
       <c r="L28" s="2" t="b">
         <v>1</v>
@@ -7227,7 +7223,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
         <v>308</v>
       </c>
       <c r="B29" t="s">
@@ -7242,7 +7238,7 @@
       <c r="E29" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="6" t="s">
         <v>341</v>
       </c>
       <c r="J29" s="2" t="str">
@@ -7251,7 +7247,7 @@
       </c>
       <c r="K29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.ReleaseMode = sNWBRest.rootObject.releaseMode.value.Truncate( 128);</v>
+        <v>this.ReleaseMode = restMain.releaseMode.value.Truncate( 128);</v>
       </c>
       <c r="L29" s="2" t="b">
         <v>1</v>
@@ -7266,7 +7262,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" t="s">
         <v>310</v>
       </c>
       <c r="B30" t="s">
@@ -7278,7 +7274,7 @@
       <c r="E30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>342</v>
       </c>
       <c r="J30" s="2" t="str">
@@ -7287,7 +7283,7 @@
       </c>
       <c r="K30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.SourceHost = sNWBRest.rootObject.sourceHost.value.Truncate( );</v>
+        <v>this.SourceHost = restMain.sourceHost.value.Truncate( );</v>
       </c>
       <c r="L30" s="2" t="b">
         <v>1</v>
@@ -7302,7 +7298,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
@@ -7314,7 +7310,7 @@
       <c r="E31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
         <v>343</v>
       </c>
       <c r="J31" s="2" t="str">
@@ -7323,7 +7319,7 @@
       </c>
       <c r="K31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.SourcePort = sNWBRest.rootObject.sourcePort.value;</v>
+        <v>this.SourcePort = restMain.sourcePort.value;</v>
       </c>
       <c r="L31" s="2" t="b">
         <v>1</v>
@@ -7338,7 +7334,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
         <v>258</v>
       </c>
       <c r="B32" t="s">
@@ -7350,7 +7346,7 @@
       <c r="E32" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="6" t="s">
         <v>279</v>
       </c>
       <c r="G32">
@@ -7368,7 +7364,7 @@
       </c>
       <c r="K32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.StreamBandwidth = sNWBRest.rootObject.streamBandwidth.value;</v>
+        <v>this.StreamBandwidth = restMain.streamBandwidth.value;</v>
       </c>
       <c r="L32" s="2" t="b">
         <v>1</v>
@@ -7383,7 +7379,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" t="s">
         <v>259</v>
       </c>
       <c r="B33" t="s">
@@ -7395,7 +7391,7 @@
       <c r="E33" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="6" t="s">
         <v>280</v>
       </c>
       <c r="J33" s="2" t="str">
@@ -7404,7 +7400,7 @@
       </c>
       <c r="K33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.StreamEnable = sNWBRest.rootObject.streamEnable.value;</v>
+        <v>this.StreamEnable = restMain.streamEnable.value;</v>
       </c>
       <c r="L33" s="2" t="b">
         <v>1</v>
@@ -7419,7 +7415,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
       <c r="B34" t="s">
@@ -7431,7 +7427,7 @@
       <c r="E34" t="s">
         <v>136</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="6" t="s">
         <v>344</v>
       </c>
       <c r="J34" s="2" t="str">
@@ -7440,7 +7436,7 @@
       </c>
       <c r="K34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.StreamId = sNWBRest.rootObject.streamId.value;</v>
+        <v>this.StreamId = restMain.streamId.value;</v>
       </c>
       <c r="L34" s="2" t="b">
         <v>1</v>
@@ -7455,7 +7451,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" t="s">
         <v>261</v>
       </c>
       <c r="B35" t="s">
@@ -7467,7 +7463,7 @@
       <c r="E35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="6" t="s">
         <v>345</v>
       </c>
       <c r="G35">
@@ -7485,7 +7481,7 @@
       </c>
       <c r="K35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.StreamSampleRate = sNWBRest.rootObject.streamSampleRate.value;</v>
+        <v>this.StreamSampleRate = restMain.streamSampleRate.value;</v>
       </c>
       <c r="L35" s="2" t="b">
         <v>1</v>
@@ -7500,7 +7496,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" t="s">
         <v>311</v>
       </c>
       <c r="B36" t="s">
@@ -7512,7 +7508,7 @@
       <c r="E36" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="6" t="s">
         <v>346</v>
       </c>
       <c r="J36" s="2" t="str">
@@ -7521,7 +7517,7 @@
       </c>
       <c r="K36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UnderflowCount = sNWBRest.rootObject.underflowCount.value;</v>
+        <v>this.UnderflowCount = restMain.underflowCount.value;</v>
       </c>
       <c r="L36" s="2" t="b">
         <v>1</v>
@@ -7536,7 +7532,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" t="s">
         <v>312</v>
       </c>
       <c r="B37" t="s">
@@ -7548,7 +7544,7 @@
       <c r="E37" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="6" t="s">
         <v>347</v>
       </c>
       <c r="J37" s="2" t="str">
@@ -7557,7 +7553,7 @@
       </c>
       <c r="K37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UpstreamIrigLocked = sNWBRest.rootObject.upstreamIrigLocked.value;</v>
+        <v>this.UpstreamIrigLocked = restMain.upstreamIrigLocked.value;</v>
       </c>
       <c r="L37" s="2" t="b">
         <v>1</v>
@@ -7572,7 +7568,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" t="s">
         <v>313</v>
       </c>
       <c r="B38" t="s">
@@ -7584,7 +7580,7 @@
       <c r="E38" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="6" t="s">
         <v>348</v>
       </c>
       <c r="J38" s="2" t="str">
@@ -7593,7 +7589,7 @@
       </c>
       <c r="K38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UpstreamOnePpsLocked = sNWBRest.rootObject.upstreamOnePpsLocked.value;</v>
+        <v>this.UpstreamOnePpsLocked = restMain.upstreamOnePpsLocked.value;</v>
       </c>
       <c r="L38" s="2" t="b">
         <v>1</v>
@@ -7608,7 +7604,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" t="s">
         <v>314</v>
       </c>
       <c r="B39" t="s">
@@ -7620,7 +7616,7 @@
       <c r="E39" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="6" t="s">
         <v>349</v>
       </c>
       <c r="J39" s="2" t="str">
@@ -7629,7 +7625,7 @@
       </c>
       <c r="K39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UpstreamPathGain = sNWBRest.rootObject.upstreamPathGain.value;</v>
+        <v>this.UpstreamPathGain = restMain.upstreamPathGain.value;</v>
       </c>
       <c r="L39" s="2" t="b">
         <v>1</v>
@@ -7644,7 +7640,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="A40" t="s">
         <v>315</v>
       </c>
       <c r="B40" t="s">
@@ -7656,7 +7652,7 @@
       <c r="E40" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="6" t="s">
         <v>350</v>
       </c>
       <c r="J40" s="2" t="str">
@@ -7665,7 +7661,7 @@
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UpstreamTenMhzLocked = sNWBRest.rootObject.upstreamTenMhzLocked.value;</v>
+        <v>this.UpstreamTenMhzLocked = restMain.upstreamTenMhzLocked.value;</v>
       </c>
       <c r="L40" s="2" t="b">
         <v>1</v>
@@ -7680,7 +7676,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>316</v>
       </c>
       <c r="B41" t="s">
@@ -7692,7 +7688,7 @@
       <c r="E41" t="s">
         <v>136</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="6" t="s">
         <v>351</v>
       </c>
       <c r="J41" s="2" t="str">
@@ -7701,7 +7697,7 @@
       </c>
       <c r="K41" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>this.UseLocalReference = sNWBRest.rootObject.useLocalReference.value;</v>
+        <v>this.UseLocalReference = restMain.useLocalReference.value;</v>
       </c>
       <c r="L41" s="2" t="b">
         <v>1</v>
@@ -7734,22 +7730,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="6"/>
-    <col min="6" max="6" width="8.88671875" style="8"/>
-    <col min="7" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="5"/>
+    <col min="6" max="6" width="8.88671875" style="6"/>
+    <col min="7" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -7787,13 +7783,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D2" s="2">
@@ -7844,19 +7840,19 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>946250474</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>264</v>
       </c>
       <c r="J3" s="2" t="str">
@@ -7895,19 +7891,19 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>265</v>
       </c>
       <c r="J4" s="2" t="str">
@@ -7931,22 +7927,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>128</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>266</v>
       </c>
       <c r="J5" s="2" t="str">
@@ -7970,19 +7966,19 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>50000</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>267</v>
       </c>
       <c r="J6" s="2" t="str">
@@ -8006,19 +8002,19 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>268</v>
       </c>
       <c r="J7" s="2" t="str">
@@ -8042,22 +8038,22 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>1500</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>270</v>
       </c>
       <c r="J8" s="2" t="str">
@@ -8081,28 +8077,28 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>946250000</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>1000000</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>262</v>
       </c>
       <c r="J9" s="2" t="str">
@@ -8126,28 +8122,28 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>78125</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>1000</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>284</v>
       </c>
       <c r="J10" s="2" t="str">
@@ -8171,28 +8167,28 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>24799.993600003203</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>1000000</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>274</v>
       </c>
       <c r="J11" s="2" t="str">
@@ -8216,22 +8212,22 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>4.8877146631439938</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>178</v>
       </c>
       <c r="J12" s="2" t="str">
@@ -8255,19 +8251,19 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6" t="b">
+      <c r="C13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>276</v>
       </c>
       <c r="J13" s="2" t="str">
@@ -8291,19 +8287,19 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>257</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>277</v>
       </c>
       <c r="J14" s="2" t="str">
@@ -8327,19 +8323,19 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>50000</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="6" t="s">
         <v>278</v>
       </c>
       <c r="J15" s="2" t="str">
@@ -8363,28 +8359,28 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>45000000</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>1000000</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>151</v>
       </c>
       <c r="J16" s="2" t="str">
@@ -8408,19 +8404,19 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6" t="b">
+      <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>280</v>
       </c>
       <c r="J17" s="2" t="str">
@@ -8444,22 +8440,22 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>148</v>
       </c>
       <c r="J18" s="2" t="str">
@@ -8483,19 +8479,19 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>282</v>
       </c>
       <c r="J19" s="2" t="str">
@@ -8519,28 +8515,28 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>50000025</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>1000000</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>152</v>
       </c>
       <c r="J20" s="2" t="str">

</xml_diff>

<commit_message>
Fixed Spectrum tables Added format and Range config tables
</commit_message>
<xml_diff>
--- a/BuildDBScript/JsonToExcel.xlsx
+++ b/BuildDBScript/JsonToExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NarrowBand\SnnbFailover\BuildDBScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774594C-5071-4EF3-9E18-E202DC4D3508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F838D48-D5BA-42DF-A9FE-0D2F0B39D584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3108" yWindow="4224" windowWidth="23040" windowHeight="12168" activeTab="3" xr2:uid="{2B70F1A1-21A2-4A0E-AB73-14BC681AD4F9}"/>
+    <workbookView xWindow="8184" yWindow="1536" windowWidth="23040" windowHeight="14424" activeTab="6" xr2:uid="{2B70F1A1-21A2-4A0E-AB73-14BC681AD4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Route" sheetId="8" r:id="rId4"/>
     <sheet name="RfOutputStream" sheetId="7" r:id="rId5"/>
     <sheet name="RfInputStream" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="FormatConfig" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">AvailableStreams!$A$1:$C$13</definedName>
@@ -33,6 +33,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -65,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="359">
   <si>
     <t>Name</t>
   </si>
@@ -1130,6 +1141,18 @@
   </si>
   <si>
     <t>destination</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>AvailableStreams</t>
+  </si>
+  <si>
+    <t>RfOutputStream</t>
+  </si>
+  <si>
+    <t>RfInputStream</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1164,8 +1187,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1173,11 +1202,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1197,19 +1250,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="54">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1236,9 +1299,6 @@
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1262,6 +1322,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="fill" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1632,7 +1701,7 @@
     <tableColumn id="10" xr3:uid="{0E8D6385-316A-409A-AC99-E8FB911598DB}" uniqueName="10" name="CapName" queryTableFieldId="10">
       <calculatedColumnFormula>UPPER(LEFT(A2,1))&amp;RIGHT(A2,LEN(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{3C1CDFAB-9FA6-49C1-9FBD-9F6A93669B16}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{3C1CDFAB-9FA6-49C1-9FBD-9F6A93669B16}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="20">
       <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = ipc.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = ipc.", A2, ".value;"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{0DEF0107-BB52-4836-86D7-F529BA9E4C3A}" uniqueName="12" name="Include" queryTableFieldId="12"/>
@@ -1666,7 +1735,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E380CAB2-72AE-4E85-91BC-EC134806B651}" name="Table_WRW_RH_SN_REST_Attr__35" displayName="Table_WRW_RH_SN_REST_Attr__35" ref="A1:N4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:N4" xr:uid="{B4DFC9B2-E0F1-4C34-81E9-BD4E969EB3FC}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{3962A823-97EE-44F4-BF9D-AE149000AE8D}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3962A823-97EE-44F4-BF9D-AE149000AE8D}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{B3F61FD9-E9C5-4318-8862-DAD6DD16EF02}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{CAD2D918-96FE-42C7-B5F6-7105062DE64B}" uniqueName="3" name="Value.value" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{2FF4556C-3C7C-443E-8824-E421486F7CAE}" uniqueName="4" name="StringLength" queryTableFieldId="4"/>
@@ -1678,7 +1747,7 @@
     <tableColumn id="10" xr3:uid="{237DF59A-1E38-445A-9CBC-64FAF55D8456}" uniqueName="10" name="CapName" queryTableFieldId="10">
       <calculatedColumnFormula>UPPER(LEFT(A2,1))&amp;RIGHT(A2,LEN(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F500B023-F33A-409C-BB73-B971BB55FBA8}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{F500B023-F33A-409C-BB73-B971BB55FBA8}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="18">
       <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = structure.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = structure.", A2, ".value;"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{35572074-5B52-405F-BB6B-7A64865B421B}" uniqueName="12" name="Include" queryTableFieldId="12"/>
@@ -1712,12 +1781,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{24D814A6-1CEC-4AEF-A328-1CD2A4C08D6D}" name="Table_RfOutputStream" displayName="Table_RfOutputStream" ref="A1:N41" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:N41" xr:uid="{24D814A6-1CEC-4AEF-A328-1CD2A4C08D6D}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6063A3EA-E7ED-4664-BF1B-624A18D1981A}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{6063A3EA-E7ED-4664-BF1B-624A18D1981A}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{5F6B9E3D-F6C7-41AB-882E-AEEB01CAA7DC}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{67043735-9D1F-4EFE-BE83-85CA3E2F8AE6}" uniqueName="3" name="Value.value" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{03F9C369-B02B-4E0A-B585-F38103A75F93}" uniqueName="4" name="StringLength" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{5DE39BA3-6B32-4E50-A22A-80B30B6DCC7C}" uniqueName="5" name="Access" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{1BDDE075-F09B-4795-B56C-0020089F2C9B}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{1BDDE075-F09B-4795-B56C-0020089F2C9B}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{DAA22772-FC2A-48E9-8EBD-CF0174760F01}" uniqueName="7" name="Scale" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{5C79966D-28ED-4B38-8DEF-162DF486CF52}" uniqueName="8" name="Format" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{A3495477-A5CF-401C-970E-7C9F91DAF030}" uniqueName="9" name="Units" queryTableFieldId="9"/>
@@ -1755,26 +1824,26 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}" name="Table_RfInputStream" displayName="Table_RfInputStream" ref="A1:N20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}" name="Table_RfInputStream" displayName="Table_RfInputStream" ref="A1:N20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:N20" xr:uid="{00E94570-A94C-4647-ACDF-085AE53491BC}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{485F7603-3220-49DD-B3CE-BFD08F35B4F8}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{321E942D-A13D-4AF0-AA77-E3500F5EB193}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{18F13399-7530-4051-8061-5D3623022EC1}" uniqueName="3" name="Value.value" queryTableFieldId="3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{8F5EA99F-A1D5-4DCA-9D86-CE635CE023A7}" uniqueName="4" name="StringLength" queryTableFieldId="4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{43FAB6A3-A2E3-48D6-B09C-12B3A53D6D11}" uniqueName="5" name="Access" queryTableFieldId="5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{522604AD-37CB-4F5E-8E4D-89F1B491602D}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{E561D537-D6AB-4F01-90DA-3BB8AB928187}" uniqueName="7" name="Scale" queryTableFieldId="7" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{106A1A6F-1D11-4875-B000-BA1B53D0CF4C}" uniqueName="8" name="Format" queryTableFieldId="8" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{84AF41AD-5261-4D2A-BC8C-68C1F8B88E4A}" uniqueName="9" name="Units" queryTableFieldId="9" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{9E5BB20E-C3F2-46F6-B5EA-7E078EB418AE}" uniqueName="10" name="CapName" queryTableFieldId="10" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{485F7603-3220-49DD-B3CE-BFD08F35B4F8}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{321E942D-A13D-4AF0-AA77-E3500F5EB193}" uniqueName="2" name="Value.factoryType" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{18F13399-7530-4051-8061-5D3623022EC1}" uniqueName="3" name="Value.value" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{8F5EA99F-A1D5-4DCA-9D86-CE635CE023A7}" uniqueName="4" name="StringLength" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{43FAB6A3-A2E3-48D6-B09C-12B3A53D6D11}" uniqueName="5" name="Access" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{522604AD-37CB-4F5E-8E4D-89F1B491602D}" uniqueName="6" name="Help" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{E561D537-D6AB-4F01-90DA-3BB8AB928187}" uniqueName="7" name="Scale" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{106A1A6F-1D11-4875-B000-BA1B53D0CF4C}" uniqueName="8" name="Format" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{84AF41AD-5261-4D2A-BC8C-68C1F8B88E4A}" uniqueName="9" name="Units" queryTableFieldId="9" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{9E5BB20E-C3F2-46F6-B5EA-7E078EB418AE}" uniqueName="10" name="CapName" queryTableFieldId="10" dataDxfId="5">
       <calculatedColumnFormula>UPPER(LEFT(A2,1))&amp;RIGHT(A2,LEN(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D10744BC-3808-4F25-B3AB-2402E774E707}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{D10744BC-3808-4F25-B3AB-2402E774E707}" uniqueName="11" name="Json-&gt;Class" queryTableFieldId="11" dataDxfId="4">
       <calculatedColumnFormula xml:space="preserve"> IF(B2 = "string", _xlfn.CONCAT("this.", J2, " = structure.", A2, ".value.Truncate( ", D2, ");"), _xlfn.CONCAT("this.", J2, " = structure.", A2, ".value;"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8219D72E-B8A2-402F-8D09-24C87022E783}" uniqueName="12" name="Include" queryTableFieldId="12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{644B8F5D-451A-40B4-8939-D1515D745218}" uniqueName="13" name="Type translate" queryTableFieldId="13" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{8219D72E-B8A2-402F-8D09-24C87022E783}" uniqueName="12" name="Include" queryTableFieldId="12" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{644B8F5D-451A-40B4-8939-D1515D745218}" uniqueName="13" name="Type translate" queryTableFieldId="13" dataDxfId="2">
       <calculatedColumnFormula>IF(B2 = "uint8", "[NUMERIC](5) NOT NULL,",
  IF(B2 = "uint16", "[NUMERIC](5) NOT NULL,",
  IF(B2 = "uint32", "[NUMERIC](10) NOT NULL,",
@@ -1792,7 +1861,7 @@
  IF(B2 = "image", "[Image] NOT NULL,",
 "")))))))))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{9EB1E7BC-2297-4F8F-B325-B0E00FD1A8AF}" uniqueName="14" name="Sql Script" queryTableFieldId="14" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{9EB1E7BC-2297-4F8F-B325-B0E00FD1A8AF}" uniqueName="14" name="Sql Script" queryTableFieldId="14" dataDxfId="1">
       <calculatedColumnFormula>IF(L2=FALSE,"",_xlfn.CONCAT("[",A2,"] ", M2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2100,8 +2169,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5374,7 +5443,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K13"/>
+      <selection activeCell="A2" sqref="A2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6166,7 +6235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D77A757-8188-4D3F-9DD3-F49E00DACB65}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
@@ -6379,7 +6448,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K41"/>
+      <selection activeCell="A2" sqref="A2:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7103,6 +7172,9 @@
       <c r="F17" s="6" t="s">
         <v>275</v>
       </c>
+      <c r="H17" t="s">
+        <v>234</v>
+      </c>
       <c r="I17" t="s">
         <v>178</v>
       </c>
@@ -8033,8 +8105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFCEDF5-23EE-4645-8BC4-22A4B8721E2C}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8043,7 +8115,7 @@
     <col min="2" max="2" width="18.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="5"/>
-    <col min="6" max="6" width="36.21875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="36.21875" style="12" customWidth="1"/>
     <col min="7" max="10" width="8.88671875" style="5"/>
     <col min="11" max="11" width="12.109375" style="5" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="5"/>
@@ -8065,7 +8137,7 @@
       <c r="E1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>137</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -8109,7 +8181,7 @@
       <c r="E2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>263</v>
       </c>
       <c r="G2" s="2"/>
@@ -8163,7 +8235,7 @@
       <c r="E3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="12" t="s">
         <v>264</v>
       </c>
       <c r="J3" s="2" t="str">
@@ -8214,7 +8286,7 @@
       <c r="E4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="12" t="s">
         <v>265</v>
       </c>
       <c r="J4" s="2" t="str">
@@ -8253,7 +8325,7 @@
       <c r="E5" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="12" t="s">
         <v>266</v>
       </c>
       <c r="J5" s="2" t="str">
@@ -8289,7 +8361,7 @@
       <c r="E6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="12" t="s">
         <v>267</v>
       </c>
       <c r="J6" s="2" t="str">
@@ -8325,7 +8397,7 @@
       <c r="E7" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="12" t="s">
         <v>268</v>
       </c>
       <c r="J7" s="2" t="str">
@@ -8361,7 +8433,7 @@
       <c r="E8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="12" t="s">
         <v>269</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -8400,7 +8472,7 @@
       <c r="E9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="12" t="s">
         <v>271</v>
       </c>
       <c r="G9" s="5">
@@ -8445,7 +8517,7 @@
       <c r="E10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="12" t="s">
         <v>272</v>
       </c>
       <c r="G10" s="5">
@@ -8490,7 +8562,7 @@
       <c r="E11" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="12" t="s">
         <v>273</v>
       </c>
       <c r="G11" s="5">
@@ -8535,7 +8607,7 @@
       <c r="E12" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="12" t="s">
         <v>275</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -8574,7 +8646,7 @@
       <c r="E13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="12" t="s">
         <v>276</v>
       </c>
       <c r="J13" s="2" t="str">
@@ -8613,7 +8685,7 @@
       <c r="E14" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="12" t="s">
         <v>277</v>
       </c>
       <c r="J14" s="2" t="str">
@@ -8649,7 +8721,7 @@
       <c r="E15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="12" t="s">
         <v>278</v>
       </c>
       <c r="J15" s="2" t="str">
@@ -8685,7 +8757,7 @@
       <c r="E16" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="12" t="s">
         <v>279</v>
       </c>
       <c r="G16" s="5">
@@ -8730,7 +8802,7 @@
       <c r="E17" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="12" t="s">
         <v>280</v>
       </c>
       <c r="J17" s="2" t="str">
@@ -8766,7 +8838,7 @@
       <c r="E18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="12" t="s">
         <v>281</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -8805,7 +8877,7 @@
       <c r="E19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="12" t="s">
         <v>282</v>
       </c>
       <c r="J19" s="2" t="str">
@@ -8841,7 +8913,7 @@
       <c r="E20" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="12" t="s">
         <v>283</v>
       </c>
       <c r="G20" s="5">
@@ -8885,13 +8957,3706 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9920F6-4A96-4263-AAD5-9492275F5A9F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="25.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="83.6640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="25.21875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10">
+        <v>128</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="10">
+        <v>128</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8">
+        <v>512</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10">
+        <v>128</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="10">
+        <v>39</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="8">
+        <v>98</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="8">
+        <v>5280</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="10">
+        <v>128</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="8">
+        <v>128</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="10">
+        <v>128</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="8">
+        <v>512</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="10">
+        <v>-10.763101577758787</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="8">
+        <v>92.783180236816406</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="10">
+        <v>128</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1421.050048828125</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="10">
+        <v>-10.763101577758787</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="8">
+        <v>92.783180236816406</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="10">
+        <v>71</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="8">
+        <v>-34.330123901367188</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="8">
+        <v>-10.629526138305664</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="10">
+        <v>92.985565185546875</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="8">
+        <v>73</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="10">
+        <v>4.8034496307373047</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="10">
+        <v>128</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="8">
+        <v>-34.330123901367188</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="10">
+        <v>60000000</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="8">
+        <v>128</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="10">
+        <v>128</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="8">
+        <v>39</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="10">
+        <v>71</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="8">
+        <v>128</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="10">
+        <v>128</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="10">
+        <v>128</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="8">
+        <v>1200</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="10">
+        <v>-60</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="8">
+        <v>18.181818008422852</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="10">
+        <v>-60</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="8">
+        <v>18.181818008422852</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="10">
+        <v>-50.241001129150391</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" s="10">
+        <v>-60</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48" s="8">
+        <v>18.181818008422852</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="10">
+        <v>-50.241001129150391</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="10">
+        <v>128</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="8">
+        <v>-50.241001129150391</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1200</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E54" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="10">
+        <v>577616640</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="8">
+        <v>1578202168</v>
+      </c>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="10">
+        <v>128</v>
+      </c>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="8">
+        <v>128</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F62" s="10">
+        <v>128</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="8">
+        <v>128</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" s="10">
+        <v>128</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F65" s="8">
+        <v>128</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E66" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E67" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E68" s="10">
+        <v>42</v>
+      </c>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" s="8">
+        <v>128</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E70" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F71" s="8">
+        <v>128</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="8">
+        <v>128</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="10">
+        <v>128</v>
+      </c>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E74" s="8">
+        <v>0</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E75" s="10">
+        <v>1200000000</v>
+      </c>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I76" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J76" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E77" s="10">
+        <v>5625000</v>
+      </c>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="8">
+        <v>10</v>
+      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E79" s="10">
+        <v>10</v>
+      </c>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E80" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E81" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E82" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E83" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="F84" s="8">
+        <v>128</v>
+      </c>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E85" s="10">
+        <v>9216000</v>
+      </c>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="J85" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E86" s="8">
+        <v>10</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F87" s="10">
+        <v>128</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E88" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I88" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="J88" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E89" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I89" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E90" s="8">
+        <v>50000</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" s="10">
+        <v>0</v>
+      </c>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E92" s="8">
+        <v>0</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J92" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E93" s="10">
+        <v>1</v>
+      </c>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E94" s="8">
+        <v>10000000</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I94" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="J94" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E95" s="10">
+        <v>118273680</v>
+      </c>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E96" s="8">
+        <v>9765</v>
+      </c>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I96" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J96" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E97" s="10">
+        <v>10</v>
+      </c>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E98" s="8">
+        <v>722559.9999999993</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="J98" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E99" s="10">
+        <v>4.8877146631439938</v>
+      </c>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I99" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F100" s="8">
+        <v>128</v>
+      </c>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E101" s="10">
+        <v>0</v>
+      </c>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E102" s="8">
+        <v>0</v>
+      </c>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E103" s="10">
+        <v>0</v>
+      </c>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E104" s="8">
+        <v>0</v>
+      </c>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E105" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E106" s="8">
+        <v>0</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1000</v>
+      </c>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E108" s="8">
+        <v>0</v>
+      </c>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E109" s="10">
+        <v>0</v>
+      </c>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E110" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F110" s="8"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="J110" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="F111" s="10">
+        <v>128</v>
+      </c>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="J111" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="8">
+        <v>128</v>
+      </c>
+      <c r="G112" s="8"/>
+      <c r="H112" s="8"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E113" s="10">
+        <v>50000</v>
+      </c>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+      <c r="I113" s="10"/>
+      <c r="J113" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E114" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H114" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I114" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J114" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E115" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="J115" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E116" s="8">
+        <v>0</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
+      <c r="J116" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E117" s="10">
+        <v>5625000</v>
+      </c>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H117" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I117" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J117" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E118" s="8">
+        <v>139</v>
+      </c>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
+      <c r="J118" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E119" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="10"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+      <c r="J119" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E120" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="8"/>
+      <c r="J120" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E121" s="10">
+        <v>10</v>
+      </c>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E122" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E123" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F124" s="8">
+        <v>128</v>
+      </c>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E125" s="10">
+        <v>946250474</v>
+      </c>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E126" s="8">
+        <v>9</v>
+      </c>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
+      <c r="I126" s="8"/>
+      <c r="J126" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C127" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F127" s="10">
+        <v>128</v>
+      </c>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E128" s="8">
+        <v>50000</v>
+      </c>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
+      <c r="J128" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E129" s="10">
+        <v>0</v>
+      </c>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E130" s="8">
+        <v>1500</v>
+      </c>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="J130" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E131" s="10">
+        <v>946250000</v>
+      </c>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H131" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I131" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="J131" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E132" s="8">
+        <v>78125</v>
+      </c>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H132" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I132" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J132" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D133" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E133" s="10">
+        <v>24799.993600003203</v>
+      </c>
+      <c r="F133" s="10"/>
+      <c r="G133" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="H133" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I133" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="J133" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E134" s="8">
+        <v>4.8877146631439938</v>
+      </c>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J134" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E135" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="J135" s="10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E136" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F136" s="8">
+        <v>128</v>
+      </c>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D137" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E137" s="10">
+        <v>50000</v>
+      </c>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E138" s="8">
+        <v>45000000</v>
+      </c>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H138" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I138" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J138" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E139" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="J139" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E140" s="8">
+        <v>0</v>
+      </c>
+      <c r="F140" s="8"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J140" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E141" s="10">
+        <v>0</v>
+      </c>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+      <c r="J141" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E142" s="8">
+        <v>50000025</v>
+      </c>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H142" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I142" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J142" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>